<commit_message>
Add image and update eval metrics
</commit_message>
<xml_diff>
--- a/results/eval-metrics.xlsx
+++ b/results/eval-metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="0" windowWidth="16820" windowHeight="17260" tabRatio="500"/>
+    <workbookView xWindow="11980" yWindow="0" windowWidth="16820" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>demo-image1</t>
   </si>
@@ -111,10 +111,13 @@
     <t>Hogwarts Express</t>
   </si>
   <si>
-    <t>training_set/21</t>
-  </si>
-  <si>
-    <t>Sunset Blcd</t>
+    <t>training_set/22</t>
+  </si>
+  <si>
+    <t>BLANK BOX</t>
+  </si>
+  <si>
+    <t>Brooklyn Bridge</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -906,18 +909,38 @@
         <v>31</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>3.5</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>1</v>
       </c>
     </row>

</xml_diff>